<commit_message>
desenho de solução e requisitos
</commit_message>
<xml_diff>
--- a/Projeto-Documentacao/Tabela de Requisitos.xlsx
+++ b/Projeto-Documentacao/Tabela de Requisitos.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Requisitos</t>
   </si>
@@ -223,18 +223,143 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Cadastro deve ter um Botão de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cadastra-se</t>
+      <t>O Software deve conter um</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'Menu'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, para opções.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O Software deve conter um campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Monitoramento'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Mostrando Graficos ao Usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O Software deve conter um campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Historico'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, que mostre ao usuario todo o controle de temperatura e umidade por dia.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O Software deve conter um campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Alerta'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, que mostre ao usuario possiveis problemas detectados.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Graficos deve mostrar taxas de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Temperatura</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Umidade</t>
     </r>
     <r>
       <rPr>
@@ -249,173 +374,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Login deve ter um Botão de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>logar-se.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>O Software deve conter um</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 'Menu'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, para opções.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O Software deve conter um campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Monitoramento'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Mostrando Graficos ao Usuario.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O Software deve conter um campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Historico'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, que mostre ao usuario todo o controle de temperatura e umidade por dia.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">O Software deve conter um campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Alerta'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, que mostre ao usuario possiveis problemas detectados.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Graficos deve mostrar taxas de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Temperatura</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Umidade</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">A Página institucional deve conter um campo  </t>
     </r>
     <r>
@@ -467,9 +425,6 @@
     </r>
   </si>
   <si>
-    <t>RF16</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">O Software deve ter um </t>
     </r>
@@ -522,9 +477,6 @@
     </r>
   </si>
   <si>
-    <t>RF17</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Alerta deve permitir que seja feito </t>
     </r>
@@ -638,12 +590,6 @@
     </r>
   </si>
   <si>
-    <t>RNF21</t>
-  </si>
-  <si>
-    <t>RNF22</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve"> É necessario um </t>
     </r>
@@ -697,6 +643,12 @@
   </si>
   <si>
     <t>Desejavel</t>
+  </si>
+  <si>
+    <t>RNF16</t>
+  </si>
+  <si>
+    <t>RNF17</t>
   </si>
 </sst>
 </file>
@@ -787,8 +739,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C23" totalsRowShown="0">
-  <autoFilter ref="A1:C23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C21" totalsRowShown="0">
+  <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Requisitos"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1095,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1190,7 +1142,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1201,10 +1153,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1214,7 +1166,7 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1223,9 +1175,9 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1234,10 +1186,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,10 +1197,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,7 +1208,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1267,10 +1219,10 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,40 +1230,40 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>8</v>
@@ -1319,7 +1271,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>41</v>
@@ -1330,35 +1282,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>